<commit_message>
data.xlsx is staged and commited
</commit_message>
<xml_diff>
--- a/Bestbuy/data.xlsx
+++ b/Bestbuy/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U14920\BestbuyDDFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vNewRepo1\Bestbuy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,9 +80,6 @@
     <t>Testcase2</t>
   </si>
   <si>
-    <t>TestCase1</t>
-  </si>
-  <si>
     <t>column1</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>Samsung</t>
+  </si>
+  <si>
+    <t>Testcase1</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,24 +621,24 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -669,10 +669,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -683,13 +683,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,31 +717,31 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>25</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>26</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -819,24 +819,24 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>36</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
       </c>
       <c r="F22" t="s">
         <v>1</v>
@@ -844,19 +844,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" t="s">
         <v>39</v>
       </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23">
         <v>8056037388</v>
@@ -864,96 +864,96 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>51</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="s">
-        <v>53</v>
-      </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
         <v>54</v>
       </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>55</v>
       </c>
-      <c r="E36" t="s">
-        <v>56</v>
-      </c>
       <c r="F36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -966,67 +966,67 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
         <v>71</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>72</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>73</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>74</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>75</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>76</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>77</v>
-      </c>
-      <c r="H44" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" t="s">
         <v>64</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>65</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>66</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" t="s">
         <v>67</v>
       </c>
-      <c r="E45" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>68</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>69</v>
-      </c>
-      <c r="H45" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>